<commit_message>
data driven approach driving data from excel driving data from parameter tag in testng.xml
</commit_message>
<xml_diff>
--- a/POMAutomation/src/main/java/com/danube/qa/data/TestData.xlsx
+++ b/POMAutomation/src/main/java/com/danube/qa/data/TestData.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11340" windowHeight="3930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13335" windowHeight="5175"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -28,28 +27,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>Tenant</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
     <t>lmenon</t>
   </si>
   <si>
     <t>Welc0me03</t>
   </si>
   <si>
-    <t>Emirates Holidays</t>
-  </si>
-  <si>
-    <t>Emirates Beta</t>
-  </si>
-  <si>
-    <t>UK - EKH Agent Desktop</t>
+    <t>Lavanya01</t>
+  </si>
+  <si>
+    <t>Adas</t>
   </si>
 </sst>
 </file>
@@ -408,52 +395,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>